<commit_message>
Ajout de la BDD (Dictionnaire, MCD, MPD)+ MaJ du RAF + Correction d'éléments HTML
</commit_message>
<xml_diff>
--- a/RAF.xlsx
+++ b/RAF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\IMIE\Campus_Contest_Adam_Dupuis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C851E0-EDDC-4624-9919-BA59FB1F6DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF40FB1-6882-4269-93B9-5A3B8740307B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Tâche</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>Retardé</t>
+  </si>
+  <si>
+    <t>RGPD</t>
+  </si>
+  <si>
+    <t>Acquisition du nom de domaine</t>
+  </si>
+  <si>
+    <t>Script de création de la BDD</t>
+  </si>
+  <si>
+    <t>Script d'alimentation de la BDD</t>
   </si>
 </sst>
 </file>
@@ -137,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -206,21 +218,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -288,10 +285,57 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -301,13 +345,52 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -315,81 +398,6 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -397,6 +405,50 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -405,76 +457,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,10 +843,10 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="25">
@@ -808,13 +865,13 @@
         <v>43819</v>
       </c>
       <c r="J4" s="26"/>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-      <c r="B5" s="37"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -823,180 +880,230 @@
       <c r="H5" s="27"/>
       <c r="I5" s="27"/>
       <c r="J5" s="28"/>
-      <c r="K5" s="33"/>
+      <c r="K5" s="31"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="22"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="10" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29"/>
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="5"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="23"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="15"/>
+      <c r="A8" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="19"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="16"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="15"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="19"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="39"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="15"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="19"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="38"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="39"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="15"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24"/>
+      <c r="B11" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="19"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="39"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="15"/>
+      <c r="A12" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="19"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="39"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="15"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="19"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="16"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="15"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="19"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="16"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="14"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="39"/>
+      <c r="B16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="14"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="40"/>
+      <c r="B17" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="14"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="24"/>
+      <c r="B18" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A15"/>
+  <mergeCells count="11">
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:D5"/>
     <mergeCell ref="E4:F5"/>
     <mergeCell ref="G4:H5"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
MaJ RAF + Formulaire de contact fonctionnel
</commit_message>
<xml_diff>
--- a/RAF.xlsx
+++ b/RAF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\IMIE\Campus_Contest_Adam_Dupuis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF40FB1-6882-4269-93B9-5A3B8740307B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B188F9-FFAA-44B4-847E-8D793E8DFFBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Tâche</t>
   </si>
@@ -69,15 +69,9 @@
     <t>Moodboard/Recherches</t>
   </si>
   <si>
-    <t>2e session</t>
-  </si>
-  <si>
     <t>Déploiement du site</t>
   </si>
   <si>
-    <t>JavaScript</t>
-  </si>
-  <si>
     <t>Prévisionnel</t>
   </si>
   <si>
@@ -94,6 +88,9 @@
   </si>
   <si>
     <t>Script d'alimentation de la BDD</t>
+  </si>
+  <si>
+    <t>PHP</t>
   </si>
 </sst>
 </file>
@@ -117,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +145,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -330,21 +333,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -448,6 +436,60 @@
       </left>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -457,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -468,34 +510,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -504,34 +553,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,68 +892,88 @@
     <col min="8" max="9" width="16.85546875" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <v>43816</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25">
+      <c r="D4" s="24"/>
+      <c r="E4" s="24">
         <v>43817</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25">
+      <c r="F4" s="24"/>
+      <c r="G4" s="24">
         <v>43818</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25">
+      <c r="H4" s="24"/>
+      <c r="I4" s="24">
         <v>43819</v>
       </c>
-      <c r="J4" s="26"/>
-      <c r="K4" s="30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="31"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="J4" s="28"/>
+      <c r="K4" s="37">
+        <v>43874</v>
+      </c>
+      <c r="L4" s="40">
+        <v>43875</v>
+      </c>
+      <c r="M4" s="34">
+        <v>43878</v>
+      </c>
+      <c r="N4" s="34">
+        <v>43879</v>
+      </c>
+      <c r="O4" s="41">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="44"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -897,14 +981,18 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="12"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="5"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -912,16 +1000,20 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="K7" s="36"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -929,14 +1021,18 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="14"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
       <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="19"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="5"/>
@@ -944,29 +1040,37 @@
       <c r="H9" s="5"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="14"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
       <c r="B10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="19"/>
+        <v>21</v>
+      </c>
+      <c r="C10" s="15"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="14"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
-      <c r="B11" s="36" t="s">
+      <c r="K10" s="45"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
+      <c r="B11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="19"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -974,16 +1078,20 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="14"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="K11" s="45"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="49"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="19"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -991,14 +1099,18 @@
       <c r="H12" s="4"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
       <c r="B13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="19"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1006,14 +1118,18 @@
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
       <c r="B14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="19"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1021,89 +1137,113 @@
       <c r="H14" s="4"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
       <c r="B15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="19"/>
+        <v>19</v>
+      </c>
+      <c r="C15" s="15"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="33"/>
       <c r="B16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="19"/>
+        <v>20</v>
+      </c>
+      <c r="C16" s="15"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="19"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="15"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="17"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="49"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27"/>
+      <c r="B18" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="49"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="15">
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A16"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:D5"/>
     <mergeCell ref="E4:F5"/>
     <mergeCell ref="G4:H5"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout possibilité pour ajouter une référence + MaJ RAF
</commit_message>
<xml_diff>
--- a/RAF.xlsx
+++ b/RAF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\IMIE\Campus_Contest_Adam_Dupuis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B188F9-FFAA-44B4-847E-8D793E8DFFBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6B1E69-E55C-4644-84C6-D96928866B8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,82 +520,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,63 +911,63 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="35">
         <v>43816</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24">
+      <c r="D4" s="35"/>
+      <c r="E4" s="35">
         <v>43817</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24">
+      <c r="F4" s="35"/>
+      <c r="G4" s="35">
         <v>43818</v>
       </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24">
+      <c r="H4" s="35"/>
+      <c r="I4" s="35">
         <v>43819</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="37">
+      <c r="J4" s="36"/>
+      <c r="K4" s="43">
         <v>43874</v>
       </c>
-      <c r="L4" s="40">
+      <c r="L4" s="29">
         <v>43875</v>
       </c>
-      <c r="M4" s="34">
+      <c r="M4" s="31">
         <v>43878</v>
       </c>
-      <c r="N4" s="34">
+      <c r="N4" s="31">
         <v>43879</v>
       </c>
-      <c r="O4" s="41">
+      <c r="O4" s="27">
         <v>43880</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="44"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="28"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="33" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -981,14 +981,14 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1000,14 +1000,14 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="36"/>
+      <c r="K7" s="21"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1021,14 +1021,14 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="45"/>
+      <c r="K8" s="23"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
@@ -1040,14 +1040,14 @@
       <c r="H9" s="5"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="45"/>
+      <c r="K9" s="23"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
@@ -1059,14 +1059,14 @@
       <c r="H10" s="11"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="45"/>
+      <c r="K10" s="23"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
       <c r="O10" s="49"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="19" t="s">
         <v>11</v>
       </c>
@@ -1078,14 +1078,14 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="45"/>
+      <c r="K11" s="23"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="40" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -1099,14 +1099,14 @@
       <c r="H12" s="4"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="47"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="25"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="7" t="s">
         <v>6</v>
       </c>
@@ -1118,14 +1118,14 @@
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="47"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="25"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="7" t="s">
         <v>7</v>
       </c>
@@ -1137,14 +1137,14 @@
       <c r="H14" s="4"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="47"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="25"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1156,14 +1156,14 @@
       <c r="H15" s="4"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="4"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1175,14 +1175,14 @@
       <c r="H16" s="4"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
-      <c r="K16" s="45"/>
+      <c r="K16" s="23"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="49"/>
+      <c r="M16" s="25"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="33" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="18" t="s">
@@ -1196,14 +1196,14 @@
       <c r="H17" s="4"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="45"/>
+      <c r="K17" s="23"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="49"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="11"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="17" t="s">
         <v>18</v>
       </c>
@@ -1215,11 +1215,11 @@
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="46"/>
+      <c r="K18" s="24"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="49"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="11"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>

</xml_diff>